<commit_message>
changed how we buy troops
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Bots\Travian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D35B71-3023-4B30-A28C-B0CF41C78210}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC0C878-C554-483B-B08B-B82CB086DEA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{705390CF-FC32-4C9B-ABF1-7644E5C5C3AB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{705390CF-FC32-4C9B-ABF1-7644E5C5C3AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Oasis" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="368">
   <si>
     <t>Oases</t>
   </si>
@@ -2954,6 +2954,62 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3420,62 +3476,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4732,22 +4732,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7698737D-84E8-4AF2-9755-E371DDB732E0}" name="Villages" displayName="Villages" ref="B2:N101" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7698737D-84E8-4AF2-9755-E371DDB732E0}" name="Villages" displayName="Villages" ref="B2:N101" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22">
   <autoFilter ref="B2:N101" xr:uid="{E70DD6E8-3F17-4193-A463-6610E91B20F1}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{AB7CF577-6E61-4CFC-983E-F11DF8A411DF}" name="DISTANCE" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{67E804B9-B263-4B93-AAFC-1AF426B10D97}" name="Coordonnées" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{4EB015F9-B075-46D8-A92C-E76B154F7036}" name="VILLAGE" dataDxfId="10" dataCellStyle="Lien hypertexte"/>
-    <tableColumn id="6" xr3:uid="{D1B93C3D-8B1C-41F4-A38D-86D9ACFF5212}" name="05-Nov" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{D97E1C3B-E675-4299-AE6A-39DD65CACA91}" name="05-Oct" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{FC5861E7-9881-4EBA-9B7F-D420A82E646D}" name="05-Sep" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{B2988A59-B3DD-46C4-8E82-01290A037CC9}" name="05-Aug" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{F2F77203-A5C1-4FFA-83D6-7D73C31B2F24}" name="05-Jul" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{9CA2C2F1-C625-46F8-835F-9E3038A1CCE8}" name="PLAYER" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{29675D41-1007-44D9-AD6B-9AE176573730}" name="CanRaid" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{0DDD18EB-CEB8-4230-ABBF-D8CBC0AAFB84}" name="TroopToSendMultiplier" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{4BDF327F-65C5-4954-B61B-BF6CB7399E2A}" name="ALLIANCE" dataDxfId="1" dataCellStyle="Lien hypertexte"/>
-    <tableColumn id="17" xr3:uid="{E412D31A-3BF4-4F4E-8539-669B4D8A22EA}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{AB7CF577-6E61-4CFC-983E-F11DF8A411DF}" name="DISTANCE" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{67E804B9-B263-4B93-AAFC-1AF426B10D97}" name="Coordonnées" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{4EB015F9-B075-46D8-A92C-E76B154F7036}" name="VILLAGE" dataDxfId="18" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="6" xr3:uid="{D1B93C3D-8B1C-41F4-A38D-86D9ACFF5212}" name="05-Nov" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{D97E1C3B-E675-4299-AE6A-39DD65CACA91}" name="05-Oct" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{FC5861E7-9881-4EBA-9B7F-D420A82E646D}" name="05-Sep" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{B2988A59-B3DD-46C4-8E82-01290A037CC9}" name="05-Aug" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{F2F77203-A5C1-4FFA-83D6-7D73C31B2F24}" name="05-Jul" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{9CA2C2F1-C625-46F8-835F-9E3038A1CCE8}" name="PLAYER" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{29675D41-1007-44D9-AD6B-9AE176573730}" name="CanRaid" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{0DDD18EB-CEB8-4230-ABBF-D8CBC0AAFB84}" name="TroopToSendMultiplier" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{4BDF327F-65C5-4954-B61B-BF6CB7399E2A}" name="ALLIANCE" dataDxfId="9" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="17" xr3:uid="{E412D31A-3BF4-4F4E-8539-669B4D8A22EA}" name="Description" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6628,7 +6628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F8A261-BA65-422E-B26D-412D101A8365}">
   <dimension ref="A1:V481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" workbookViewId="0">
+    <sheetView topLeftCell="A335" workbookViewId="0">
       <selection activeCell="I348" sqref="I348"/>
     </sheetView>
   </sheetViews>
@@ -15646,37 +15646,37 @@
     <sortCondition ref="F5:F63"/>
   </sortState>
   <conditionalFormatting sqref="G10:H10 G14:H14 G16:H16 G20:H20 G23:H23 G5:H5 G7:H8 G9 G11:G13 G15 G17:G19 G21:G22 G24:G63 E5:E64">
-    <cfRule type="expression" dxfId="23" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>IF(E5="false",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="expression" dxfId="22" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>IF(G6="false",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="expression" dxfId="21" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>IF(G25="false",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U4:U36">
-    <cfRule type="expression" dxfId="20" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>IF(U4="false",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4 V6:V23 V25:V36">
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>IF(V4="false",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V5">
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>IF(V5="false",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V24">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>IF(V24="false",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19301,7 +19301,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3:K101">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>IF(K3="false",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20005,10 +20005,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58BAFAA-1352-4B86-B4DE-F1EE12D71509}">
-  <dimension ref="D2:H34"/>
+  <dimension ref="D2:H38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20530,6 +20530,46 @@
         <v>4542</v>
       </c>
     </row>
+    <row r="36" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="4:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="67" t="s">
+        <v>363</v>
+      </c>
+      <c r="E37" s="66">
+        <v>9</v>
+      </c>
+      <c r="F37" s="66">
+        <f t="shared" ref="F37:H37" si="6">VLOOKUP($D37,Animals,F$15,FALSE)*$E37</f>
+        <v>2250</v>
+      </c>
+      <c r="G37" s="66">
+        <f t="shared" si="6"/>
+        <v>1260</v>
+      </c>
+      <c r="H37" s="66">
+        <f t="shared" si="6"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="66"/>
+      <c r="E38" s="69">
+        <f>SUM(E35:E37)</f>
+        <v>9</v>
+      </c>
+      <c r="F38" s="69">
+        <f>SUM(F35:F37)</f>
+        <v>2250</v>
+      </c>
+      <c r="G38" s="69">
+        <f>SUM(G35:G37)</f>
+        <v>1260</v>
+      </c>
+      <c r="H38" s="69">
+        <f>SUM(H35:H37)</f>
+        <v>1800</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added VETERAN to farm
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Bots\Travian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2CA706-FA4A-473B-BB2F-8A5720785820}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CAA959-16F8-40D0-81C8-34409A675B64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{705390CF-FC32-4C9B-ABF1-7644E5C5C3AB}"/>
   </bookViews>
@@ -15393,8 +15393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF22575-6A1A-4F29-8B52-FC457B6C6596}">
   <dimension ref="B1:V701"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D664" workbookViewId="0">
-      <selection activeCell="M684" sqref="M684"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19533,7 +19533,7 @@
         <v>317</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L73" s="13" t="str">
         <f>SUBSTITUTE(LEFT(Villages[[#This Row],[Coordonnées]],SEARCH("|",Villages[[#This Row],[Coordonnées]])-1),"(","")</f>
@@ -26524,11 +26524,11 @@
       </c>
       <c r="S496" t="str">
         <f>INDEX(Villages[],Q496,10)</f>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="V496" t="str">
         <f>CHAR(34)&amp;R496&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;S496&amp;CHAR(34)&amp;","</f>
-        <v>"CanRaid": "false",</v>
+        <v>"CanRaid": "true",</v>
       </c>
     </row>
     <row r="497" spans="17:22" x14ac:dyDescent="0.25">

</xml_diff>